<commit_message>
Updated 134,137 test data sheet and IS functions
</commit_message>
<xml_diff>
--- a/Test Data/TC_134_Verify_IB_Units_On_Assigning_Base_And_Additional_Base.xlsx
+++ b/Test Data/TC_134_Verify_IB_Units_On_Assigning_Base_And_Additional_Base.xlsx
@@ -325,7 +325,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -335,6 +334,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -635,12 +635,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="17"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -721,7 +721,7 @@
       <c r="H7" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="17" t="s">
         <v>43</v>
       </c>
     </row>
@@ -751,7 +751,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="I8" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -780,7 +780,7 @@
         <v>7.7</v>
       </c>
       <c r="I9" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -809,7 +809,7 @@
         <v>11.8</v>
       </c>
       <c r="I10" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -842,12 +842,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="17"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">

</xml_diff>

<commit_message>
Updated base change test case data
</commit_message>
<xml_diff>
--- a/Test Data/TC_134_Verify_IB_Units_On_Assigning_Base_And_Additional_Base.xlsx
+++ b/Test Data/TC_134_Verify_IB_Units_On_Assigning_Base_And_Additional_Base.xlsx
@@ -30,8 +30,114 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Alpesh Dhakad</author>
+  </authors>
+  <commentList>
+    <comment ref="D8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Alpesh Dhakad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+801SB [516.800.907] @ 90dB</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Alpesh Dhakad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+801RB [516.800.905]</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Alpesh Dhakad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+801RB [516.800.905]</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Alpesh Dhakad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+801RB [516.800.905]</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="46">
   <si>
     <t>Device</t>
   </si>
@@ -163,13 +269,19 @@
   </si>
   <si>
     <t>IBUnitsLoadingDetail</t>
+  </si>
+  <si>
+    <t>Additonal Base Row</t>
+  </si>
+  <si>
+    <t>Assign Base/Default Base Row</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,6 +303,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -225,7 +350,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -285,22 +410,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -325,7 +439,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -614,11 +727,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="I8" sqref="I8:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -635,12 +748,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="17"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -707,13 +820,13 @@
         <v>1</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>23</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>28</v>
@@ -721,7 +834,7 @@
       <c r="H7" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="5" t="s">
         <v>43</v>
       </c>
     </row>
@@ -735,14 +848,14 @@
       <c r="C8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>26</v>
+      <c r="D8" s="7">
+        <v>17</v>
       </c>
       <c r="E8" s="7">
-        <v>13</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>24</v>
+        <v>6</v>
+      </c>
+      <c r="F8" s="7">
+        <v>1</v>
       </c>
       <c r="G8" s="7">
         <v>6</v>
@@ -750,7 +863,7 @@
       <c r="H8" s="3">
         <v>5.0999999999999996</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="11" t="s">
         <v>39</v>
       </c>
     </row>
@@ -764,11 +877,11 @@
       <c r="C9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>24</v>
+      <c r="D9" s="7">
+        <v>39</v>
       </c>
       <c r="E9" s="7">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>3</v>
@@ -779,7 +892,7 @@
       <c r="H9" s="3">
         <v>7.7</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="11" t="s">
         <v>39</v>
       </c>
     </row>
@@ -797,10 +910,10 @@
         <v>3</v>
       </c>
       <c r="E10" s="7">
-        <v>13</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>24</v>
+        <v>6</v>
+      </c>
+      <c r="F10" s="7">
+        <v>1</v>
       </c>
       <c r="G10" s="7">
         <v>6</v>
@@ -808,7 +921,7 @@
       <c r="H10" s="3">
         <v>11.8</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="11" t="s">
         <v>39</v>
       </c>
     </row>
@@ -818,6 +931,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -842,12 +956,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="17"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">

</xml_diff>